<commit_message>
add finetuning results for gpt4o and gpt4.1
</commit_message>
<xml_diff>
--- a/Results/real_clocks/Test_Llama-3.2-11B-Vision-Instruct_Train_Results.xlsx
+++ b/Results/real_clocks/Test_Llama-3.2-11B-Vision-Instruct_Train_Results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,1717 +453,2227 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01:09</t>
+          <t>01:08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **07:02:59**.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>07:02:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>01:32</t>
+          <t>01:09</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:02**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>10:02</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>01:49</t>
+          <t>01:15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:00**.</t>
+          <t>The time shown on the clock is **04:01:01**.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>04:01:01</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>01:49</t>
+          <t>01:18</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **04:01:01**.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>04:01:01</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01:50</t>
+          <t>01:25</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **05:01:01**.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>05:01:01</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:00</t>
+          <t>01:32</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:00**.</t>
+          <t>The time shown on the clock is **06:01:01**.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>06:01:01</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:07</t>
+          <t>01:49</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:08**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>10:08</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>02:13</t>
+          <t>01:49</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:02**.</t>
+          <t>The time shown on the clock is **08:01:59**.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10:02</t>
+          <t>08:01:59</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>02:14</t>
+          <t>01:50</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:55**.</t>
+          <t>The time shown on the clock is **10:00:00**.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>10:55</t>
+          <t>10:00:00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>02:25</t>
+          <t>02:00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>02:26</t>
+          <t>02:07</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **12:00:08**.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>12:00:08</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>02:27</t>
+          <t>02:13</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **08:01:59**.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>08:01:59</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>02:39</t>
+          <t>02:14</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:55**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>11:55</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>02:41</t>
+          <t>02:22</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:52**.</t>
+          <t>The time shown on the clock is **04:01:01**.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>04:01:01</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03:00</t>
+          <t>02:25</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:00**.</t>
+          <t>The time shown on the clock is **05:54:01**.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>05:54:01</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>02:26</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **05:24:59**.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>05:24:59</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>03:09</t>
+          <t>02:27</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **01:19:59**.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>01:19:59</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03:31</t>
+          <t>02:39</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:55**.</t>
+          <t>The time shown on the clock is **01:24:59**.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>11:55</t>
+          <t>01:24:59</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03:32</t>
+          <t>02:40</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **06:01:01**.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>06:01:01</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03:36</t>
+          <t>02:41</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:08**.</t>
+          <t>The time shown on the clock is **01:24:59**.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10:08</t>
+          <t>01:24:59</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>03:47</t>
+          <t>02:51</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:52**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>03:47</t>
+          <t>03:00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:52**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:58</t>
+          <t>03:02</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:22**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>11:22</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:00</t>
+          <t>03:09</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **01:01:01**.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>01:01:01</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>04:26</t>
+          <t>03:16</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **01:01:24**.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>01:01:24</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>04:32</t>
+          <t>03:29</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **05:59:59**.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>05:59:59</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:34</t>
+          <t>03:31</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **06:00:00**.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>06:00:00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>05:01</t>
+          <t>03:32</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:02**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>10:02</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>05:02</t>
+          <t>03:36</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:54**.</t>
+          <t>The time shown on the clock is **01:59:59**.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>11:54</t>
+          <t>01:59:59</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>05:05</t>
+          <t>03:47</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:52**.</t>
+          <t>The time shown on the clock is **01:01:24**.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>01:01:24</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>05:20</t>
+          <t>03:47</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **01:01:43**.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>01:01:43</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05:30</t>
+          <t>03:58</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **07:01:59**.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>07:01:59</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:02**.</t>
+          <t>The time shown on the clock is **08:01:59**.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10:02</t>
+          <t>08:01:59</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:52</t>
+          <t>04:16</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **01:01:58**.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>01:01:58</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:53</t>
+          <t>04:26</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>04:32</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:00**.</t>
+          <t>The time shown on the clock is **01:43:59**.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>01:43:59</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>04:34</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:52**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>06:05</t>
+          <t>04:59</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:12**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>11:12</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>06:12</t>
+          <t>05:01</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:12</t>
+          <t>05:02</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **12:00:00**.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>12:00:00</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:35</t>
+          <t>05:05</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:04**.</t>
+          <t>The time shown on the clock is **07:02:59**.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>10:04</t>
+          <t>07:02:59</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:36</t>
+          <t>05:20</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **04:01:24**.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>04:01:24</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:49</t>
+          <t>05:30</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **05:59:59**.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>05:59:59</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **01:01:43**.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>01:01:43</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>05:52</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>07:09</t>
+          <t>05:53</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **06:01:01**.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>06:01:01</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>07:14</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **06:00:00**.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>06:00:00</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **01:15:08**.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>01:15:08</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>07:27</t>
+          <t>06:05</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:54**.</t>
+          <t>The time shown on the clock is **07:01:59**.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11:54</t>
+          <t>07:01:59</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>07:46</t>
+          <t>06:12</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **06:01:59**.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>06:01:59</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>07:52</t>
+          <t>06:12</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **06:01:24**.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>06:01:24</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>07:58</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:30**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>08:14</t>
+          <t>06:35</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **06:01:24**.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>06:01:24</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:18</t>
+          <t>06:36</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:00**.</t>
+          <t>The time shown on the clock is **07:01:59**.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>07:01:59</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>06:49</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:08**.</t>
+          <t>The time shown on the clock is **01:18:59**.</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10:08</t>
+          <t>01:18:59</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>08:48</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:55**.</t>
+          <t>The time shown on the clock is **07:01:59**.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>10:55</t>
+          <t>07:01:59</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:55**.</t>
+          <t>The time shown on the clock is **06:01:59**.</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>10:55</t>
+          <t>06:01:59</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:08**.</t>
+          <t>The time shown on the clock is **01:24:59**.</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10:08</t>
+          <t>01:24:59</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>08:59</t>
+          <t>07:09</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **01:24:59**.</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>01:24:59</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>09:05</t>
+          <t>07:12</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:00**.</t>
+          <t>The time shown on the clock is **01:01:43**.</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>01:01:43</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>07:14</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **01:01:43**.</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>01:01:43</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **07:02:59**.</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>07:02:59</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>09:13</t>
+          <t>07:27</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **07:02:59**.</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>07:02:59</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>09:19</t>
+          <t>07:46</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>07:52</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:58**.</t>
+          <t>The time shown on the clock is **01:01:24**.</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>01:01:24</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>07:55</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:52**.</t>
+          <t>The time shown on the clock is **06:01:59**.</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>06:01:59</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>09:29</t>
+          <t>07:58</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:08**.</t>
+          <t>The time shown on the clock is **01:24:59**.</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>10:08</t>
+          <t>01:24:59</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>09:38</t>
+          <t>08:14</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:11**.</t>
+          <t>The time shown on the clock is **08:01:24**.</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>11:11</t>
+          <t>08:01:24</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>09:50</t>
+          <t>08:14</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:46**.</t>
+          <t>The time shown on the clock is **08:01:01**.</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>11:46</t>
+          <t>08:01:01</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>09:55</t>
+          <t>08:18</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:08**.</t>
+          <t>The time shown on the clock is **08:01:01**.</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>10:08</t>
+          <t>08:01:01</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>10:08</t>
+          <t>08:22</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **01:58:01**.</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>01:58:01</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>08:27</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **01:01:24**.</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>01:01:24</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>08:47</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **01:24:59**.</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>01:24:59</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>10:11</t>
+          <t>08:48</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:30**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>10:14</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:52**.</t>
+          <t>The time shown on the clock is **01:01:43**.</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>01:01:43</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>10:16</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:09**.</t>
+          <t>The time shown on the clock is **01:15:59**.</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>10:09</t>
+          <t>01:15:59</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>08:59</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:00**.</t>
+          <t>The time shown on the clock is **11:02:59**.</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:02:59</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>10:32</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:52**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>10:48</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:21**.</t>
+          <t>The time shown on the clock is **08:01:24**.</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>08:01:24</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>10:51</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:52**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>11:13</t>
+          <t>09:12</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:55**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>11:55</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **02:01:59**.</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>02:01:59</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>11:29</t>
+          <t>09:19</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **06:01:01**.</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>06:01:01</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:08**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10:08</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **08:01:24**.</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>08:01:24</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>09:29</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **07:01:59**.</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>07:01:59</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:00**.</t>
+          <t>The time shown on the clock is **01:01:01**.</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>01:01:01</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:50</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:18**.</t>
+          <t>The time shown on the clock is **01:18:59**.</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>11:18</t>
+          <t>01:18:59</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>12:01</t>
+          <t>09:55</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:46**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>11:46</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>12:03</t>
+          <t>10:08</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:52**.</t>
+          <t>The time shown on the clock is **10:02:59**.</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>10:02:59</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>12:04</t>
+          <t>10:08</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:00**.</t>
+          <t>The time shown on the clock is **10:02:59**.</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:02:59</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>10:09</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>10:10</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:12**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>11:12</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>12:24</t>
+          <t>10:10</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:08**.</t>
+          <t>The time shown on the clock is **10:02:59**.</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>10:08</t>
+          <t>10:02:59</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>12:27</t>
+          <t>10:10</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:00**.</t>
+          <t>The time shown on the clock is **06:01:24**.</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>06:01:24</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>10:11</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:03**.</t>
+          <t>The time shown on the clock is **01:24:59**.</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>01:24:59</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>12:40</t>
+          <t>10:14</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **10:10**.</t>
+          <t>The time shown on the clock is **01:01:59**.</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>01:01:59</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>12:54</t>
+          <t>10:16</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:50**.</t>
+          <t>The time shown on the clock is **10:00:00**.</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>10:00:00</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>12:55</t>
+          <t>10:21</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:00**.</t>
+          <t>The time shown on the clock is **06:01:24**.</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>06:01:24</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>12:55</t>
+          <t>10:32</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>The time shown on the clock is **11:00**.</t>
+          <t>The time shown on the clock is **07:01:01**.</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>07:01:01</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
+          <t>10:34</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **12:00:00**.</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>10:40</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **08:01:01**.</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>08:01:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>10:48</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **12:01:24**.</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>12:01:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>10:51</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **06:01:59**.</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>06:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>10:57</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>10:59</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **12:00:08**.</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>12:00:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **12:00:00**.</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>11:13</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **05:01:14**.</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>05:01:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>11:29</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **06:00:00**.</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>06:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>11:37</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:24:59**.</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>01:24:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **12:00:00**.</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **06:00:00**.</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>06:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>12:01</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>12:03</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **12:00:00**.</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **12:00:00**.</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>12:24</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>12:27</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>12:31</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:14:59**.</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>01:14:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **07:01:01**.</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>07:01:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>12:40</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:59**.</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>01:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>12:54</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **01:01:01**.</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>01:01:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>12:55</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **11:01:01**.</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>11:01:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>12:55</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **06:00:00**.</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>06:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
           <t>12:59</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>The time shown on the clock is **10:00**.</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>10:00</t>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>The time shown on the clock is **12:00:00**.</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
         </is>
       </c>
     </row>

</xml_diff>